<commit_message>
Hoàn thiện chức năng tạo mới sản phẩm Thêm mới chức năng tạo nhóm hàng
</commit_message>
<xml_diff>
--- a/api/APIs.xlsx
+++ b/api/APIs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrblu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\Startup\IPOS\api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1FEEACF-A8EE-46DE-9C74-5DBD36F9CC73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EEFB2861-56FA-45DE-B610-9CF6CDB95950}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{FDAE5902-28A3-4E45-8196-0DE845D5B61C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Product</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Tạo mã giao dịch (truyền vào loại giao dịch, vd : I, B, M, …)</t>
+  </si>
+  <si>
+    <t>ExportFile</t>
+  </si>
+  <si>
+    <t>Export data ra file xlsx, lưu trên thư mục ExportFiles (temp)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,8 +514,12 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>

</xml_diff>